<commit_message>
End Of Line Edge Case added.
</commit_message>
<xml_diff>
--- a/States M1.xlsx
+++ b/States M1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="342">
   <si>
     <t>Y0Y1</t>
   </si>
@@ -736,19 +736,336 @@
   </si>
   <si>
     <t>G5B5</t>
+  </si>
+  <si>
+    <t>U1+U6</t>
+  </si>
+  <si>
+    <t>U2+U5</t>
+  </si>
+  <si>
+    <t>U3+U4</t>
+  </si>
+  <si>
+    <t>V1+V6</t>
+  </si>
+  <si>
+    <t>V2+V5</t>
+  </si>
+  <si>
+    <t>V3+V4</t>
+  </si>
+  <si>
+    <t>U'6=U3</t>
+  </si>
+  <si>
+    <t>U'7</t>
+  </si>
+  <si>
+    <t>V'6=V3</t>
+  </si>
+  <si>
+    <t>V'7</t>
+  </si>
+  <si>
+    <t>U158U159</t>
+  </si>
+  <si>
+    <t>V158V159</t>
+  </si>
+  <si>
+    <t>U159</t>
+  </si>
+  <si>
+    <t>V159</t>
+  </si>
+  <si>
+    <t>U158</t>
+  </si>
+  <si>
+    <t>U157</t>
+  </si>
+  <si>
+    <t>U156</t>
+  </si>
+  <si>
+    <t>U155</t>
+  </si>
+  <si>
+    <t>U154</t>
+  </si>
+  <si>
+    <t>U153</t>
+  </si>
+  <si>
+    <t>V153</t>
+  </si>
+  <si>
+    <t>V154</t>
+  </si>
+  <si>
+    <t>V155</t>
+  </si>
+  <si>
+    <t>V156</t>
+  </si>
+  <si>
+    <t>U153+U158</t>
+  </si>
+  <si>
+    <t>U154+U157</t>
+  </si>
+  <si>
+    <t>U155+U156</t>
+  </si>
+  <si>
+    <t>V153+V158</t>
+  </si>
+  <si>
+    <t>V154+V157</t>
+  </si>
+  <si>
+    <t>U'310=U155</t>
+  </si>
+  <si>
+    <t>U'311</t>
+  </si>
+  <si>
+    <t>V'311</t>
+  </si>
+  <si>
+    <t>Y310</t>
+  </si>
+  <si>
+    <t>Y310Y311</t>
+  </si>
+  <si>
+    <t>Y311</t>
+  </si>
+  <si>
+    <t>Y310-16</t>
+  </si>
+  <si>
+    <t>V'310-128</t>
+  </si>
+  <si>
+    <t>U'310-128</t>
+  </si>
+  <si>
+    <t>Y311-16</t>
+  </si>
+  <si>
+    <t>V'311-128</t>
+  </si>
+  <si>
+    <t>U'311-128</t>
+  </si>
+  <si>
+    <t>U160U161</t>
+  </si>
+  <si>
+    <t>V160V161</t>
+  </si>
+  <si>
+    <t>V157</t>
+  </si>
+  <si>
+    <t>V158</t>
+  </si>
+  <si>
+    <t>V155+V156</t>
+  </si>
+  <si>
+    <t>V'310=C155</t>
+  </si>
+  <si>
+    <t>R310=mult1+mult2</t>
+  </si>
+  <si>
+    <t>G310=mult1-mult2-mult3</t>
+  </si>
+  <si>
+    <t>B310=mult1+mult3</t>
+  </si>
+  <si>
+    <t>R310G310</t>
+  </si>
+  <si>
+    <t>G311B311</t>
+  </si>
+  <si>
+    <t>R311=mult1+mult2</t>
+  </si>
+  <si>
+    <t>G311=mult1-mult2-mult3</t>
+  </si>
+  <si>
+    <t>B311=mult1+mult3</t>
+  </si>
+  <si>
+    <t>B310R311</t>
+  </si>
+  <si>
+    <t>Y312Y313</t>
+  </si>
+  <si>
+    <t>U154+U159</t>
+  </si>
+  <si>
+    <t>U155+U158</t>
+  </si>
+  <si>
+    <t>U156+U157</t>
+  </si>
+  <si>
+    <t>U'312=U156</t>
+  </si>
+  <si>
+    <t>U'313</t>
+  </si>
+  <si>
+    <t>V154+V159</t>
+  </si>
+  <si>
+    <t>V155+V158</t>
+  </si>
+  <si>
+    <t>V156+V157</t>
+  </si>
+  <si>
+    <t>V'312=V156</t>
+  </si>
+  <si>
+    <t>V'313</t>
+  </si>
+  <si>
+    <t>Y312-16</t>
+  </si>
+  <si>
+    <t>V'312-128</t>
+  </si>
+  <si>
+    <t>U'312-128</t>
+  </si>
+  <si>
+    <t>U'313-128</t>
+  </si>
+  <si>
+    <t>V'313-128</t>
+  </si>
+  <si>
+    <t>Y313-16</t>
+  </si>
+  <si>
+    <t>G312=mult1-mult2-mult3</t>
+  </si>
+  <si>
+    <t>B312=mult1+mult3</t>
+  </si>
+  <si>
+    <t>R312=mult1+mult2</t>
+  </si>
+  <si>
+    <t>R313=mult1+mult2</t>
+  </si>
+  <si>
+    <t>G313=mult1-mult2-mult3</t>
+  </si>
+  <si>
+    <t>B313=mult1+mult3</t>
+  </si>
+  <si>
+    <t>Y312</t>
+  </si>
+  <si>
+    <t>Y313</t>
+  </si>
+  <si>
+    <t>R312G312</t>
+  </si>
+  <si>
+    <t>B312R313</t>
+  </si>
+  <si>
+    <t>G313B313</t>
+  </si>
+  <si>
+    <t>R316G316</t>
+  </si>
+  <si>
+    <t>B316R317</t>
+  </si>
+  <si>
+    <t>G317B317</t>
+  </si>
+  <si>
+    <t>Y317-16</t>
+  </si>
+  <si>
+    <t>V'317-128</t>
+  </si>
+  <si>
+    <t>U'317-128</t>
+  </si>
+  <si>
+    <t>G316=mult1-mult2-mult3</t>
+  </si>
+  <si>
+    <t>R317=mult1+mult2</t>
+  </si>
+  <si>
+    <t>B317=mult1+mult3</t>
+  </si>
+  <si>
+    <t>U'317</t>
+  </si>
+  <si>
+    <t>G317=mult1-mult2-mult3</t>
+  </si>
+  <si>
+    <t>R316=mult1+mult2</t>
+  </si>
+  <si>
+    <t>B316=mult1+mult3</t>
+  </si>
+  <si>
+    <t>U'316-128</t>
+  </si>
+  <si>
+    <t>V'316-128</t>
+  </si>
+  <si>
+    <t>U162U163</t>
+  </si>
+  <si>
+    <t>V162V163</t>
+  </si>
+  <si>
+    <t>GOTO STATE G</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -785,6 +1102,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -813,7 +1136,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -823,6 +1146,16 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1746,11 +2079,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AK42"/>
+  <dimension ref="A1:AY42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="R1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AC34" sqref="AC34"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="AR1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AY10" sqref="AY10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1771,21 +2104,30 @@
     <col min="24" max="24" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="9.140625" style="10"/>
     <col min="30" max="30" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="12.42578125" style="8" customWidth="1"/>
-    <col min="32" max="32" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="32" max="33" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="15.7109375" customWidth="1"/>
     <col min="35" max="35" width="20.7109375" customWidth="1"/>
-    <col min="36" max="36" width="16.140625" customWidth="1"/>
-    <col min="37" max="37" width="21.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="16.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="11" bestFit="1" customWidth="1"/>
     <col min="40" max="40" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="41" max="41" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="17" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="21.85546875" bestFit="1" customWidth="1"/>
     <col min="43" max="43" width="22" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="21.85546875" customWidth="1"/>
+    <col min="47" max="47" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="23.140625" customWidth="1"/>
+    <col min="50" max="50" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1829,7 +2171,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1896,8 +2238,24 @@
       <c r="Z2">
         <v>146952</v>
       </c>
-    </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AI2">
+        <v>156</v>
+      </c>
+      <c r="AM2">
+        <v>38480</v>
+      </c>
+      <c r="AN2">
+        <v>38481</v>
+      </c>
+      <c r="AO2">
+        <v>57880</v>
+      </c>
+      <c r="AS2">
+        <v>57881</v>
+      </c>
+      <c r="AU2" s="9"/>
+    </row>
+    <row r="3" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1937,8 +2295,34 @@
       <c r="Z3" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AD3" s="9" t="s">
+        <v>250</v>
+      </c>
+      <c r="AE3" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="AF3" s="9" t="s">
+        <v>273</v>
+      </c>
+      <c r="AI3" s="9"/>
+      <c r="AL3" s="9" t="s">
+        <v>296</v>
+      </c>
+      <c r="AP3" s="9" t="s">
+        <v>281</v>
+      </c>
+      <c r="AQ3" s="9" t="s">
+        <v>339</v>
+      </c>
+      <c r="AR3" s="9" t="s">
+        <v>282</v>
+      </c>
+      <c r="AT3" s="9"/>
+      <c r="AU3" s="9"/>
+      <c r="AX3" s="9"/>
+      <c r="AY3" s="9"/>
+    </row>
+    <row r="4" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1969,8 +2353,36 @@
       <c r="Z4" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AJ4" s="9" t="s">
+        <v>290</v>
+      </c>
+      <c r="AK4" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="AL4" s="9" t="s">
+        <v>291</v>
+      </c>
+      <c r="AP4" s="9" t="s">
+        <v>321</v>
+      </c>
+      <c r="AQ4" s="9" t="s">
+        <v>322</v>
+      </c>
+      <c r="AR4" s="9" t="s">
+        <v>323</v>
+      </c>
+      <c r="AS4" s="9"/>
+      <c r="AV4" s="9" t="s">
+        <v>324</v>
+      </c>
+      <c r="AW4" s="9" t="s">
+        <v>325</v>
+      </c>
+      <c r="AX4" s="9" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="5" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1995,8 +2407,20 @@
       <c r="AA5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AI5">
+        <v>0</v>
+      </c>
+      <c r="AJ5">
+        <v>1</v>
+      </c>
+      <c r="AP5">
+        <v>1</v>
+      </c>
+      <c r="AV5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -2006,8 +2430,15 @@
       <c r="Y6" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AE6" s="11"/>
+      <c r="AQ6" s="9" t="s">
+        <v>281</v>
+      </c>
+      <c r="AY6" s="14" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="7" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -2017,23 +2448,38 @@
       <c r="Z7" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AF7" s="9" t="s">
+        <v>253</v>
+      </c>
+      <c r="AS7" s="9" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="8" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AE9" s="11" t="s">
+        <v>252</v>
+      </c>
+      <c r="AR9" s="9" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="10" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AT10" s="9" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="11" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>34</v>
       </c>
@@ -2046,8 +2492,16 @@
       <c r="S11" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AF11" s="9"/>
+      <c r="AG11" s="9" t="s">
+        <v>272</v>
+      </c>
+      <c r="AM11" s="9" t="s">
+        <v>319</v>
+      </c>
+      <c r="AP11" s="9"/>
+    </row>
+    <row r="12" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>35</v>
       </c>
@@ -2060,8 +2514,16 @@
       <c r="S12" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="13" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AF12" s="9"/>
+      <c r="AG12" s="9" t="s">
+        <v>274</v>
+      </c>
+      <c r="AM12" s="9" t="s">
+        <v>320</v>
+      </c>
+      <c r="AP12" s="9"/>
+    </row>
+    <row r="13" spans="1:51" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>26</v>
       </c>
@@ -2092,8 +2554,21 @@
       <c r="Y13" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AE13" s="9" t="s">
+        <v>259</v>
+      </c>
+      <c r="AF13" s="8"/>
+      <c r="AJ13" s="9" t="s">
+        <v>258</v>
+      </c>
+      <c r="AP13" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="AV13" s="9" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="14" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>27</v>
       </c>
@@ -2124,8 +2599,21 @@
       <c r="Y14" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AE14" s="9" t="s">
+        <v>258</v>
+      </c>
+      <c r="AF14" s="8"/>
+      <c r="AJ14" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="AP14" s="9" t="s">
+        <v>256</v>
+      </c>
+      <c r="AV14" s="9" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="15" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>28</v>
       </c>
@@ -2156,8 +2644,21 @@
       <c r="Y15" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AE15" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="AF15" s="8"/>
+      <c r="AJ15" s="9" t="s">
+        <v>256</v>
+      </c>
+      <c r="AP15" s="9" t="s">
+        <v>255</v>
+      </c>
+      <c r="AV15" s="9" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="16" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>29</v>
       </c>
@@ -2188,8 +2689,21 @@
       <c r="Y16" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AE16" s="9" t="s">
+        <v>256</v>
+      </c>
+      <c r="AF16" s="8"/>
+      <c r="AJ16" s="9" t="s">
+        <v>255</v>
+      </c>
+      <c r="AP16" s="9" t="s">
+        <v>254</v>
+      </c>
+      <c r="AV16" s="9" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="17" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>30</v>
       </c>
@@ -2217,8 +2731,21 @@
       <c r="Y17" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AE17" s="9" t="s">
+        <v>255</v>
+      </c>
+      <c r="AF17" s="8"/>
+      <c r="AJ17" s="9" t="s">
+        <v>254</v>
+      </c>
+      <c r="AP17" s="9" t="s">
+        <v>252</v>
+      </c>
+      <c r="AV17" s="9" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="18" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>31</v>
       </c>
@@ -2246,18 +2773,35 @@
       <c r="Y18" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AE18" s="9" t="s">
+        <v>254</v>
+      </c>
+      <c r="AF18" s="8"/>
+      <c r="AJ18" s="9" t="s">
+        <v>252</v>
+      </c>
+      <c r="AP18" s="9" t="s">
+        <v>252</v>
+      </c>
+      <c r="AV18" s="9" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="19" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AE19"/>
+      <c r="AF19" s="8"/>
+    </row>
+    <row r="20" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AE20"/>
+      <c r="AF20" s="8"/>
+    </row>
+    <row r="21" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -2282,8 +2826,21 @@
       <c r="Z21" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AE21"/>
+      <c r="AF21" s="11" t="s">
+        <v>260</v>
+      </c>
+      <c r="AK21" s="11" t="s">
+        <v>261</v>
+      </c>
+      <c r="AQ21" s="9" t="s">
+        <v>262</v>
+      </c>
+      <c r="AW21" s="9" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="22" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -2308,8 +2865,21 @@
       <c r="Z22" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AE22"/>
+      <c r="AF22" s="11" t="s">
+        <v>261</v>
+      </c>
+      <c r="AK22" s="11" t="s">
+        <v>262</v>
+      </c>
+      <c r="AQ22" s="9" t="s">
+        <v>263</v>
+      </c>
+      <c r="AW22" s="9" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="23" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -2334,8 +2904,21 @@
       <c r="Z23" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AE23"/>
+      <c r="AF23" s="11" t="s">
+        <v>262</v>
+      </c>
+      <c r="AK23" s="11" t="s">
+        <v>263</v>
+      </c>
+      <c r="AQ23" s="9" t="s">
+        <v>283</v>
+      </c>
+      <c r="AW23" s="9" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="24" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -2360,8 +2943,25 @@
       <c r="Z24" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AE24"/>
+      <c r="AF24" s="11" t="s">
+        <v>263</v>
+      </c>
+      <c r="AK24" s="11" t="s">
+        <v>283</v>
+      </c>
+      <c r="AQ24" s="9" t="s">
+        <v>284</v>
+      </c>
+      <c r="AT24" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="AU24" s="13"/>
+      <c r="AW24" s="9" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="25" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -2383,8 +2983,21 @@
       <c r="Z25" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AE25"/>
+      <c r="AF25" s="11" t="s">
+        <v>283</v>
+      </c>
+      <c r="AK25" s="11" t="s">
+        <v>284</v>
+      </c>
+      <c r="AQ25" s="9" t="s">
+        <v>253</v>
+      </c>
+      <c r="AW25" s="9" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="26" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -2403,18 +3016,31 @@
       <c r="Z26" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AE26"/>
+      <c r="AF26" s="11" t="s">
+        <v>284</v>
+      </c>
+      <c r="AK26" s="11" t="s">
+        <v>253</v>
+      </c>
+      <c r="AQ26" s="9" t="s">
+        <v>253</v>
+      </c>
+      <c r="AW26" s="9" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="27" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>37</v>
       </c>
@@ -2454,8 +3080,42 @@
       <c r="X29">
         <v>72684</v>
       </c>
-    </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="Z29">
+        <v>21</v>
+      </c>
+      <c r="AA29">
+        <v>21</v>
+      </c>
+      <c r="AF29">
+        <v>21</v>
+      </c>
+      <c r="AG29">
+        <v>21</v>
+      </c>
+      <c r="AH29">
+        <v>72684</v>
+      </c>
+      <c r="AJ29">
+        <v>72684</v>
+      </c>
+      <c r="AK29"/>
+      <c r="AL29">
+        <v>21</v>
+      </c>
+      <c r="AM29">
+        <v>21</v>
+      </c>
+      <c r="AN29">
+        <v>72684</v>
+      </c>
+      <c r="AP29">
+        <v>72684</v>
+      </c>
+      <c r="AV29">
+        <v>72684</v>
+      </c>
+    </row>
+    <row r="30" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>38</v>
       </c>
@@ -2495,8 +3155,47 @@
       <c r="X30" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="Z30" s="9" t="s">
+        <v>240</v>
+      </c>
+      <c r="AA30" s="9" t="s">
+        <v>243</v>
+      </c>
+      <c r="AF30" s="9" t="s">
+        <v>264</v>
+      </c>
+      <c r="AG30" s="9" t="s">
+        <v>267</v>
+      </c>
+      <c r="AH30" s="9" t="s">
+        <v>275</v>
+      </c>
+      <c r="AJ30" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="AK30"/>
+      <c r="AL30" s="9" t="s">
+        <v>297</v>
+      </c>
+      <c r="AM30" s="9" t="s">
+        <v>302</v>
+      </c>
+      <c r="AN30" s="9" t="s">
+        <v>307</v>
+      </c>
+      <c r="AP30" s="9" t="s">
+        <v>312</v>
+      </c>
+      <c r="AR30" s="9"/>
+      <c r="AS30" s="9"/>
+      <c r="AV30" s="9" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="31" spans="1:49" x14ac:dyDescent="0.2">
+      <c r="AK31"/>
+    </row>
+    <row r="32" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>39</v>
       </c>
@@ -2554,8 +3253,59 @@
       <c r="Y32">
         <v>25624</v>
       </c>
-    </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="Z32">
+        <v>52</v>
+      </c>
+      <c r="AA32">
+        <v>52</v>
+      </c>
+      <c r="AF32">
+        <v>52</v>
+      </c>
+      <c r="AG32">
+        <v>52</v>
+      </c>
+      <c r="AH32">
+        <v>104595</v>
+      </c>
+      <c r="AI32">
+        <v>25624</v>
+      </c>
+      <c r="AJ32">
+        <v>104595</v>
+      </c>
+      <c r="AK32">
+        <v>25624</v>
+      </c>
+      <c r="AL32">
+        <v>52</v>
+      </c>
+      <c r="AM32">
+        <v>52</v>
+      </c>
+      <c r="AN32">
+        <v>104595</v>
+      </c>
+      <c r="AO32">
+        <v>25624</v>
+      </c>
+      <c r="AP32">
+        <v>104595</v>
+      </c>
+      <c r="AQ32">
+        <v>25624</v>
+      </c>
+      <c r="AU32">
+        <v>25624</v>
+      </c>
+      <c r="AV32">
+        <v>104595</v>
+      </c>
+      <c r="AW32">
+        <v>25624</v>
+      </c>
+    </row>
+    <row r="33" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>40</v>
       </c>
@@ -2613,8 +3363,62 @@
       <c r="Y33" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="Z33" s="9" t="s">
+        <v>241</v>
+      </c>
+      <c r="AA33" s="9" t="s">
+        <v>244</v>
+      </c>
+      <c r="AF33" s="9" t="s">
+        <v>265</v>
+      </c>
+      <c r="AG33" s="9" t="s">
+        <v>268</v>
+      </c>
+      <c r="AH33" s="9" t="s">
+        <v>276</v>
+      </c>
+      <c r="AI33" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="AJ33" s="9" t="s">
+        <v>279</v>
+      </c>
+      <c r="AK33" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="AL33" s="9" t="s">
+        <v>298</v>
+      </c>
+      <c r="AM33" s="9" t="s">
+        <v>303</v>
+      </c>
+      <c r="AN33" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="AO33" s="9" t="s">
+        <v>309</v>
+      </c>
+      <c r="AP33" s="9" t="s">
+        <v>311</v>
+      </c>
+      <c r="AQ33" s="9" t="s">
+        <v>310</v>
+      </c>
+      <c r="AU33" s="9" t="s">
+        <v>337</v>
+      </c>
+      <c r="AV33" s="9" t="s">
+        <v>328</v>
+      </c>
+      <c r="AW33" s="9" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="34" spans="1:50" x14ac:dyDescent="0.2">
+      <c r="AK34"/>
+    </row>
+    <row r="35" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>41</v>
       </c>
@@ -2672,8 +3476,59 @@
       <c r="Y35">
         <v>53281</v>
       </c>
-    </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="Z35">
+        <v>159</v>
+      </c>
+      <c r="AA35">
+        <v>159</v>
+      </c>
+      <c r="AF35">
+        <v>159</v>
+      </c>
+      <c r="AG35">
+        <v>159</v>
+      </c>
+      <c r="AH35">
+        <v>132251</v>
+      </c>
+      <c r="AI35">
+        <v>53281</v>
+      </c>
+      <c r="AJ35">
+        <v>132251</v>
+      </c>
+      <c r="AK35">
+        <v>53281</v>
+      </c>
+      <c r="AL35">
+        <v>159</v>
+      </c>
+      <c r="AM35">
+        <v>159</v>
+      </c>
+      <c r="AN35">
+        <v>132251</v>
+      </c>
+      <c r="AO35">
+        <v>53281</v>
+      </c>
+      <c r="AP35">
+        <v>132251</v>
+      </c>
+      <c r="AQ35">
+        <v>53281</v>
+      </c>
+      <c r="AU35">
+        <v>53281</v>
+      </c>
+      <c r="AV35">
+        <v>132251</v>
+      </c>
+      <c r="AW35">
+        <v>53281</v>
+      </c>
+    </row>
+    <row r="36" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>42</v>
       </c>
@@ -2731,8 +3586,59 @@
       <c r="Y36" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="Z36" s="9" t="s">
+        <v>242</v>
+      </c>
+      <c r="AA36" s="9" t="s">
+        <v>245</v>
+      </c>
+      <c r="AF36" s="9" t="s">
+        <v>266</v>
+      </c>
+      <c r="AG36" s="9" t="s">
+        <v>285</v>
+      </c>
+      <c r="AH36" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="AI36" s="9" t="s">
+        <v>276</v>
+      </c>
+      <c r="AJ36" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="AK36" s="9" t="s">
+        <v>279</v>
+      </c>
+      <c r="AL36" s="9" t="s">
+        <v>299</v>
+      </c>
+      <c r="AM36" s="9" t="s">
+        <v>304</v>
+      </c>
+      <c r="AN36" s="9" t="s">
+        <v>309</v>
+      </c>
+      <c r="AO36" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="AP36" s="9" t="s">
+        <v>310</v>
+      </c>
+      <c r="AQ36" s="9" t="s">
+        <v>311</v>
+      </c>
+      <c r="AU36" s="9" t="s">
+        <v>338</v>
+      </c>
+      <c r="AV36" s="9" t="s">
+        <v>329</v>
+      </c>
+      <c r="AW36" s="9" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="38" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>94</v>
       </c>
@@ -2754,8 +3660,26 @@
       <c r="U38" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="Z38" s="9" t="s">
+        <v>246</v>
+      </c>
+      <c r="AA38" s="9" t="s">
+        <v>247</v>
+      </c>
+      <c r="AF38" s="9" t="s">
+        <v>269</v>
+      </c>
+      <c r="AG38" s="9" t="s">
+        <v>270</v>
+      </c>
+      <c r="AL38" s="9" t="s">
+        <v>300</v>
+      </c>
+      <c r="AM38" s="9" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="39" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>95</v>
       </c>
@@ -2777,8 +3701,26 @@
       <c r="V39" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA39" s="9" t="s">
+        <v>248</v>
+      </c>
+      <c r="AB39" s="9" t="s">
+        <v>249</v>
+      </c>
+      <c r="AG39" s="9" t="s">
+        <v>286</v>
+      </c>
+      <c r="AH39" s="9" t="s">
+        <v>271</v>
+      </c>
+      <c r="AM39" s="9" t="s">
+        <v>305</v>
+      </c>
+      <c r="AN39" s="9" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="40" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>47</v>
       </c>
@@ -2800,8 +3742,26 @@
       <c r="Y40" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AI40" s="9" t="s">
+        <v>287</v>
+      </c>
+      <c r="AK40" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="AO40" s="9" t="s">
+        <v>315</v>
+      </c>
+      <c r="AQ40" s="9" t="s">
+        <v>316</v>
+      </c>
+      <c r="AU40" s="9" t="s">
+        <v>335</v>
+      </c>
+      <c r="AW40" s="9" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="41" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>48</v>
       </c>
@@ -2823,8 +3783,28 @@
       <c r="Z41" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AJ41" s="9" t="s">
+        <v>288</v>
+      </c>
+      <c r="AK41"/>
+      <c r="AL41" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="AP41" s="9" t="s">
+        <v>313</v>
+      </c>
+      <c r="AR41" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="AS41" s="9"/>
+      <c r="AV41" s="9" t="s">
+        <v>330</v>
+      </c>
+      <c r="AX41" s="9" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="42" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>49</v>
       </c>
@@ -2845,11 +3825,30 @@
       </c>
       <c r="Y42" t="s">
         <v>228</v>
+      </c>
+      <c r="AI42" s="9" t="s">
+        <v>289</v>
+      </c>
+      <c r="AK42" s="9" t="s">
+        <v>294</v>
+      </c>
+      <c r="AO42" s="9" t="s">
+        <v>314</v>
+      </c>
+      <c r="AQ42" s="9" t="s">
+        <v>318</v>
+      </c>
+      <c r="AU42" s="9" t="s">
+        <v>336</v>
+      </c>
+      <c r="AW42" s="9" t="s">
+        <v>332</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Few more State Changes.
</commit_message>
<xml_diff>
--- a/States M1.xlsx
+++ b/States M1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="355">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="358">
   <si>
     <t>Y0Y1</t>
   </si>
@@ -1081,6 +1081,15 @@
   </si>
   <si>
     <t>GOTO STATE B</t>
+  </si>
+  <si>
+    <t>Y314Y315</t>
+  </si>
+  <si>
+    <t>Y314</t>
+  </si>
+  <si>
+    <t>Y315</t>
   </si>
 </sst>
 </file>
@@ -2121,8 +2130,8 @@
   <dimension ref="A1:BA38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="AG1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AH8" sqref="AH8"/>
+      <pane xSplit="1" topLeftCell="AK1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AM22" sqref="AM22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2358,6 +2367,9 @@
       <c r="AK2">
         <v>156</v>
       </c>
+      <c r="AQ2">
+        <v>157</v>
+      </c>
       <c r="AW2" s="9"/>
     </row>
     <row r="3" spans="1:53" x14ac:dyDescent="0.2">
@@ -2415,7 +2427,9 @@
       </c>
       <c r="AR3" s="9"/>
       <c r="AS3" s="9"/>
-      <c r="AT3" s="9"/>
+      <c r="AT3" s="9" t="s">
+        <v>355</v>
+      </c>
       <c r="AV3" s="9"/>
       <c r="AW3" s="9"/>
       <c r="AZ3" s="9"/>
@@ -2594,6 +2608,9 @@
         <v>313</v>
       </c>
       <c r="AR11" s="9"/>
+      <c r="AU11" s="9" t="s">
+        <v>356</v>
+      </c>
     </row>
     <row r="12" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
@@ -2616,6 +2633,9 @@
         <v>314</v>
       </c>
       <c r="AR12" s="9"/>
+      <c r="AU12" s="9" t="s">
+        <v>357</v>
+      </c>
     </row>
     <row r="13" spans="1:53" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">

</xml_diff>

<commit_message>
Lab work for Nov 15
Must fix col count to restart properly (lin count too), move write data
to always comb, add stuff to reset so no more red lines in waves
modelsim. degbuuuuuug.
</commit_message>
<xml_diff>
--- a/States M1.xlsx
+++ b/States M1.xlsx
@@ -2130,8 +2130,8 @@
   <dimension ref="A1:BA38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="AK1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AM22" sqref="AM22"/>
+      <pane xSplit="1" topLeftCell="AG1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AI5" sqref="AI5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Nov 19 Lab Changes.
</commit_message>
<xml_diff>
--- a/States M1.xlsx
+++ b/States M1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="358">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="358">
   <si>
     <t>Y0Y1</t>
   </si>
@@ -2130,8 +2130,8 @@
   <dimension ref="A1:BA38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="AG1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AI5" sqref="AI5"/>
+      <pane xSplit="1" topLeftCell="AJ1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AK1" sqref="AK1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2139,10 +2139,10 @@
     <col min="1" max="1" width="15.42578125" customWidth="1"/>
     <col min="7" max="8" width="9.42578125" customWidth="1"/>
     <col min="9" max="9" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="19.7109375" bestFit="1" customWidth="1"/>
@@ -3179,9 +3179,15 @@
       <c r="J25">
         <v>72684</v>
       </c>
+      <c r="K25">
+        <v>72684</v>
+      </c>
       <c r="L25">
         <v>72684</v>
       </c>
+      <c r="M25">
+        <v>72684</v>
+      </c>
       <c r="N25">
         <v>21</v>
       </c>
@@ -3203,7 +3209,13 @@
       <c r="V25">
         <v>72684</v>
       </c>
+      <c r="W25">
+        <v>72684</v>
+      </c>
       <c r="X25">
+        <v>72684</v>
+      </c>
+      <c r="Y25">
         <v>72684</v>
       </c>
       <c r="Z25">
@@ -3260,9 +3272,15 @@
       <c r="J26" t="s">
         <v>163</v>
       </c>
+      <c r="K26" t="s">
+        <v>163</v>
+      </c>
       <c r="L26" t="s">
         <v>169</v>
       </c>
+      <c r="M26" t="s">
+        <v>169</v>
+      </c>
       <c r="N26" t="s">
         <v>181</v>
       </c>
@@ -3284,7 +3302,13 @@
       <c r="V26" t="s">
         <v>214</v>
       </c>
+      <c r="W26" t="s">
+        <v>214</v>
+      </c>
       <c r="X26" t="s">
+        <v>217</v>
+      </c>
+      <c r="Y26" t="s">
         <v>217</v>
       </c>
       <c r="Z26" s="9" t="s">
@@ -3905,10 +3929,10 @@
       <c r="A36" t="s">
         <v>43</v>
       </c>
-      <c r="K36" t="s">
+      <c r="J36" t="s">
         <v>166</v>
       </c>
-      <c r="M36" t="s">
+      <c r="L36" t="s">
         <v>172</v>
       </c>
       <c r="Q36" t="s">
@@ -3946,10 +3970,10 @@
       <c r="A37" t="s">
         <v>44</v>
       </c>
-      <c r="L37" t="s">
+      <c r="K37" t="s">
         <v>168</v>
       </c>
-      <c r="N37" t="s">
+      <c r="M37" t="s">
         <v>174</v>
       </c>
       <c r="R37" t="s">
@@ -3989,10 +4013,10 @@
       <c r="A38" t="s">
         <v>45</v>
       </c>
-      <c r="K38" t="s">
+      <c r="J38" t="s">
         <v>167</v>
       </c>
-      <c r="M38" t="s">
+      <c r="L38" t="s">
         <v>173</v>
       </c>
       <c r="Q38" t="s">

</xml_diff>

<commit_message>
November 20 EOD Commit
Problems: Column ending prematurely, skewing picture; colourspace
conversion wrong (closer then before); Confirm if we write RGB [7:0] or
[15:8]; also conversion from signed/unsigned (U', V', to RGB)
</commit_message>
<xml_diff>
--- a/States M1.xlsx
+++ b/States M1.xlsx
@@ -2133,8 +2133,8 @@
   <dimension ref="A1:BB38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="AQ1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AV22" sqref="AV22"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="K36" sqref="K36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Nov 21- After Lab Commmit
CHECK PPM. There is a misalignment when reading the Y values.
We have to properly check to make sure the values being read in are
given enough time to be used.
The column error still exists. It's skipping a few of the end pixels,
causing the the next line pixels to be used to the picture.
</commit_message>
<xml_diff>
--- a/States M1.xlsx
+++ b/States M1.xlsx
@@ -2133,8 +2133,8 @@
   <dimension ref="A1:BB38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="K36" sqref="K36"/>
+      <pane xSplit="1" topLeftCell="AQ1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AV22" sqref="AV22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>